<commit_message>
Se reaizan pruebas de acceso y mapa
</commit_message>
<xml_diff>
--- a/Documentacion Tecnica/Guiones de prueba/EM-Acceso/QA-EM-Acceso-CU1_RegistrarNuevoUsuario.xlsx
+++ b/Documentacion Tecnica/Guiones de prueba/EM-Acceso/QA-EM-Acceso-CU1_RegistrarNuevoUsuario.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidPC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W8.1\Desktop\ESCOMobile TT2\ESCOMobile\Documentacion Tecnica\Guiones de prueba\EM-Acceso\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A49843-0208-4468-A0C8-6C25325D9812}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CU1Información general" sheetId="1" r:id="rId1"/>
     <sheet name="CU1RegistrarNuevoUsuario" sheetId="2" r:id="rId2"/>
     <sheet name="EM-Acceso-CU1RegistrarNuevoUsua" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -647,7 +648,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3266,15 +3267,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor theme="9"/>
+    <tabColor rgb="FFFFC000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3577,13 +3578,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -3968,14 +3969,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AH40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>